<commit_message>
Repo Archivos SQL y de admin - Subida de respaldo
Se agregan al reporcitorio nuevos archivos y modificaciones a los que se
ejecutan diaro, si tiene dudas ya saben dond encontrarme.
</commit_message>
<xml_diff>
--- a/PedidoCubrebocas.xlsx
+++ b/PedidoCubrebocas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git\CapacitacionDesarrollo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA08C129-607F-47A0-8BAB-A81E21BEF2D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08D53A0F-43D8-4854-89CD-05150125488A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{E1F5AFB3-F2B0-4814-9DA7-0A37809772B4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="21">
   <si>
     <t>Nombre</t>
   </si>
@@ -67,13 +67,43 @@
   </si>
   <si>
     <t>Progrmación y Desrrollo</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t># De Empleado</t>
+  </si>
+  <si>
+    <t>Supervisor/ Jefe de área</t>
+  </si>
+  <si>
+    <t>Área</t>
+  </si>
+  <si>
+    <t>Rafael Eduardo Méndez Pérez</t>
+  </si>
+  <si>
+    <t>Grajales Diaz Jonatan Geovanni</t>
+  </si>
+  <si>
+    <t>Desarrollo</t>
+  </si>
+  <si>
+    <t>Miguel Alejandro Hernandez Rodrigez</t>
+  </si>
+  <si>
+    <t>--------------</t>
+  </si>
+  <si>
+    <t>--------------------------------------------------</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -94,6 +124,12 @@
       <name val="Abadi Extra Light"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -109,7 +145,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -132,19 +168,98 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -460,28 +575,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20A49287-18A2-4247-B9A0-AF888447A503}">
-  <dimension ref="B2:E11"/>
+  <dimension ref="B2:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17:E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="36.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="47.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
       <c r="E2" s="3">
-        <v>44399</v>
+        <v>44438</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
@@ -491,7 +606,7 @@
       <c r="C6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="4" t="s">
         <v>2</v>
       </c>
       <c r="E6" s="2" t="s">
@@ -505,7 +620,9 @@
       <c r="C7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="1"/>
+      <c r="D7" s="5">
+        <v>2</v>
+      </c>
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
@@ -515,7 +632,9 @@
       <c r="C8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="1"/>
+      <c r="D8" s="5">
+        <v>2</v>
+      </c>
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
@@ -525,7 +644,9 @@
       <c r="C9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="1"/>
+      <c r="D9" s="5">
+        <v>2</v>
+      </c>
       <c r="E9" s="1"/>
     </row>
     <row r="10" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
@@ -535,7 +656,9 @@
       <c r="C10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="1"/>
+      <c r="D10" s="5">
+        <v>2</v>
+      </c>
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
@@ -545,8 +668,109 @@
       <c r="C11" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="1"/>
+      <c r="D11" s="5" t="s">
+        <v>11</v>
+      </c>
       <c r="E11" s="1"/>
+    </row>
+    <row r="16" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="2:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="10">
+        <v>911328288</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="10">
+        <v>911328834</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="10">
+        <v>911318257</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="10">
+        <v>911289379</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="10">
+        <v>438</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>